<commit_message>
Formatted files and added credentials
Formatted all files for consistency and added the credentials for this assignment. Moved #include statements for sstream and fstream in all BarcodeScanner files to the Scanner files.
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sherpa/Documents/Code/GitHub/Assignment5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sherpa/Documents/School/CS 300/Assignment5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2659DE6-F67B-304F-AFDC-376B8A90F37E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86370FB-7452-2A4B-81B6-F2D1730B3F6B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="460" windowWidth="24660" windowHeight="14600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3356,7 +3356,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1117600</xdr:colOff>
+      <xdr:colOff>1422400</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
@@ -3400,7 +3400,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1117600</xdr:colOff>
+      <xdr:colOff>1422400</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -3732,7 +3732,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C2" sqref="C2:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>